<commit_message>
datos not clean Celulares_Biobio v1
</commit_message>
<xml_diff>
--- a/Exel_import/data_not_clean/Celulares_Biobio.xlsx
+++ b/Exel_import/data_not_clean/Celulares_Biobio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Desktop\CAFTON\JUNJI\inventario-junji\Exel_import\data_not_clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A3FF26-0241-4B6A-8E0F-16A67378D51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EE1FED-2FE8-4A32-8CEB-F36156884C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Celulares_Biobio" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'Celulares_Biobio'!$A$1:$S$6</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'Celulares_Biobio'!$A$1:$L$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
   <si>
     <t>Código Inventario</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Tipo Adquisición</t>
   </si>
   <si>
-    <t>Contrato</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
     <t>Número de Serie</t>
   </si>
   <si>
@@ -62,18 +56,6 @@
     <t>Modelo</t>
   </si>
   <si>
-    <t>Región</t>
-  </si>
-  <si>
-    <t>Comuna</t>
-  </si>
-  <si>
-    <t>Dependencia</t>
-  </si>
-  <si>
-    <t>Dirección</t>
-  </si>
-  <si>
     <t>Persona Asignada Actual</t>
   </si>
   <si>
@@ -86,9 +68,6 @@
     <t>Código Proveedor</t>
   </si>
   <si>
-    <t>Datos adjuntos</t>
-  </si>
-  <si>
     <t>txtMarca</t>
   </si>
   <si>
@@ -101,12 +80,6 @@
     <t>Arriendo</t>
   </si>
   <si>
-    <t>Contrato 87</t>
-  </si>
-  <si>
-    <t>EN USO</t>
-  </si>
-  <si>
     <t>R9WX30GBSLN</t>
   </si>
   <si>
@@ -116,18 +89,6 @@
     <t>Galaxy A05</t>
   </si>
   <si>
-    <t>REGION DEL BIOBIO</t>
-  </si>
-  <si>
-    <t>CONCEPCION</t>
-  </si>
-  <si>
-    <t>Oficina</t>
-  </si>
-  <si>
-    <t>O Higgins Poniente 77, piso 4, Concepción.</t>
-  </si>
-  <si>
     <t>MARIO LOPEZ</t>
   </si>
   <si>
@@ -156,6 +117,15 @@
   </si>
   <si>
     <t>SIMON CIFUENTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unidad </t>
+  </si>
+  <si>
+    <t>Direccion Regional</t>
+  </si>
+  <si>
+    <t>unidad id</t>
   </si>
 </sst>
 </file>
@@ -198,19 +168,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -262,55 +220,54 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{5C4C353D-DE31-46F4-8A76-86A6CC019DC9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="20">
-    <queryTableFields count="19">
+  <queryTableRefresh nextId="22" unboundColumnsRight="2">
+    <queryTableFields count="14">
       <queryTableField id="1" name="Código Inventario" tableColumnId="1"/>
       <queryTableField id="2" name="Tipo Dispositivo" tableColumnId="2"/>
       <queryTableField id="3" name="Tipo Adquisición" tableColumnId="3"/>
-      <queryTableField id="4" name="Contrato" tableColumnId="4"/>
-      <queryTableField id="5" name="Estado" tableColumnId="5"/>
       <queryTableField id="6" name="Número de Serie" tableColumnId="6"/>
       <queryTableField id="7" name="Marca" tableColumnId="7"/>
       <queryTableField id="8" name="Modelo" tableColumnId="8"/>
-      <queryTableField id="9" name="Región" tableColumnId="9"/>
-      <queryTableField id="10" name="Comuna" tableColumnId="10"/>
-      <queryTableField id="11" name="Dependencia" tableColumnId="11"/>
-      <queryTableField id="12" name="Dirección" tableColumnId="12"/>
       <queryTableField id="13" name="Persona Asignada Actual" tableColumnId="13"/>
       <queryTableField id="14" name="Responsable" tableColumnId="14"/>
       <queryTableField id="15" name="OC:OC" tableColumnId="15"/>
       <queryTableField id="16" name="Código Proveedor" tableColumnId="16"/>
-      <queryTableField id="17" name="Datos adjuntos" tableColumnId="17"/>
       <queryTableField id="18" name="txtMarca" tableColumnId="18"/>
       <queryTableField id="19" name="txtModelo" tableColumnId="19"/>
+      <queryTableField id="20" dataBound="0" tableColumnId="4"/>
+      <queryTableField id="21" dataBound="0" tableColumnId="5"/>
     </queryTableFields>
+    <queryTableDeletedFields count="7">
+      <deletedField name="Contrato"/>
+      <deletedField name="Estado"/>
+      <deletedField name="Región"/>
+      <deletedField name="Comuna"/>
+      <deletedField name="Dependencia"/>
+      <deletedField name="Dirección"/>
+      <deletedField name="Datos adjuntos"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E30BAAD7-0195-4931-94DE-93CA07932B43}" name="Celulares_Biobio" displayName="Celulares_Biobio" ref="A1:S6" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:S6" xr:uid="{E30BAAD7-0195-4931-94DE-93CA07932B43}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E30BAAD7-0195-4931-94DE-93CA07932B43}" name="Celulares_Biobio" displayName="Celulares_Biobio" ref="A1:N6" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:N6" xr:uid="{E30BAAD7-0195-4931-94DE-93CA07932B43}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{CD475147-A928-48FF-A1F9-211C77467A3A}" uniqueName="1" name="Código Inventario" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{9DAEAFC1-2911-434F-A7B7-9E8E68F479D3}" uniqueName="2" name="Tipo Dispositivo" queryTableFieldId="2" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{B1016E1A-C1EF-494C-8CC7-77E86968F76B}" uniqueName="3" name="Tipo Adquisición" queryTableFieldId="3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{9AFA5993-91F0-4856-9CB0-016FC6164D3D}" uniqueName="4" name="Contrato" queryTableFieldId="4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{FF137885-893D-423C-B3E1-AAA4BFFAB187}" uniqueName="5" name="Estado" queryTableFieldId="5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{8FE2AD92-7A18-4472-83E2-E76021B41A33}" uniqueName="6" name="Número de Serie" queryTableFieldId="6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{14F233F7-4E11-4C70-9B60-6AA5328A4890}" uniqueName="7" name="Marca" queryTableFieldId="7" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{CE4298E7-DDF7-499E-BEBA-2BC19DD3FD39}" uniqueName="8" name="Modelo" queryTableFieldId="8" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{99920CF4-41FA-4B6E-AFE0-DBA598BEECC3}" uniqueName="9" name="Región" queryTableFieldId="9" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{B997187A-C896-4F24-A594-C11CD9F91AAA}" uniqueName="10" name="Comuna" queryTableFieldId="10" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{A38BDB55-CD14-4299-93FF-DD141BAA2AF1}" uniqueName="11" name="Dependencia" queryTableFieldId="11" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{BEEB6B83-64B9-48D9-A09B-66C783B14D48}" uniqueName="12" name="Dirección" queryTableFieldId="12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{69474F62-261F-42A9-AB8C-DF029BE2FD01}" uniqueName="13" name="Persona Asignada Actual" queryTableFieldId="13" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{F949276B-DC3D-49F6-8E32-0F4486C49E80}" uniqueName="14" name="Responsable" queryTableFieldId="14" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{1CCE4431-0175-41C0-B7BF-54CFDFDB5D0B}" uniqueName="15" name="OC:OC" queryTableFieldId="15" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9DAEAFC1-2911-434F-A7B7-9E8E68F479D3}" uniqueName="2" name="Tipo Dispositivo" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B1016E1A-C1EF-494C-8CC7-77E86968F76B}" uniqueName="3" name="Tipo Adquisición" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{8FE2AD92-7A18-4472-83E2-E76021B41A33}" uniqueName="6" name="Número de Serie" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{14F233F7-4E11-4C70-9B60-6AA5328A4890}" uniqueName="7" name="Marca" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{CE4298E7-DDF7-499E-BEBA-2BC19DD3FD39}" uniqueName="8" name="Modelo" queryTableFieldId="8" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{69474F62-261F-42A9-AB8C-DF029BE2FD01}" uniqueName="13" name="Persona Asignada Actual" queryTableFieldId="13" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{F949276B-DC3D-49F6-8E32-0F4486C49E80}" uniqueName="14" name="Responsable" queryTableFieldId="14" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{1CCE4431-0175-41C0-B7BF-54CFDFDB5D0B}" uniqueName="15" name="OC:OC" queryTableFieldId="15" dataDxfId="4"/>
     <tableColumn id="16" xr3:uid="{E3302200-F1B6-46E0-B242-CB44F1064C82}" uniqueName="16" name="Código Proveedor" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{32EFD7A2-0577-4AF2-9F92-3F7747C2942F}" uniqueName="17" name="Datos adjuntos" queryTableFieldId="17"/>
-    <tableColumn id="18" xr3:uid="{8B77D5A8-D656-4ACE-8586-38D529C71D5F}" uniqueName="18" name="txtMarca" queryTableFieldId="18" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{DFEE9255-244E-47EA-BDA5-E438A2622D50}" uniqueName="19" name="txtModelo" queryTableFieldId="19" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{8B77D5A8-D656-4ACE-8586-38D529C71D5F}" uniqueName="18" name="txtMarca" queryTableFieldId="18" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{DFEE9255-244E-47EA-BDA5-E438A2622D50}" uniqueName="19" name="txtModelo" queryTableFieldId="19" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{51CE86AC-787E-4D07-9B7D-AF392007AB10}" uniqueName="4" name="unidad " queryTableFieldId="20" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{36086B3E-9CF7-433B-98D3-AD7B4BF90BB7}" uniqueName="5" name="unidad id" queryTableFieldId="21" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,34 +536,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A99740-FBE3-4DC3-A809-A6CF99855F83}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,320 +597,230 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>17022668</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
+        <v>56935679415</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2">
-        <v>56935679415</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>25</v>
+      <c r="N2" s="1">
+        <v>8101098</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>17022644</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>56935690973</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3">
-        <v>56935690973</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>25</v>
+      <c r="N3" s="1">
+        <v>8101098</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>17022672</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>56935691301</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4">
-        <v>56935691301</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>25</v>
+      <c r="N4" s="1">
+        <v>8101098</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>17022716</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>56989663037</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5">
-        <v>56989663037</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>25</v>
+      <c r="N5" s="1">
+        <v>8101098</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>17022679</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>56989662646</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6">
-        <v>56989662646</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>25</v>
+      <c r="N6" s="1">
+        <v>8101098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>